<commit_message>
old files into old folder. USETHIS is correct file with 10 solutions
</commit_message>
<xml_diff>
--- a/group property parameter table.xlsx
+++ b/group property parameter table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Imperial College London\School Work\Year 4\Advanced Process Optimisation\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="8_{54E9388B-7918-4662-9941-0F89BA9963D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{819F8A53-126D-4ECD-9D92-F5C197FEC32A}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="8_{54E9388B-7918-4662-9941-0F89BA9963D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8DEC40D6-E60C-468B-ABA0-02BB387D6AF8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A3056EDA-ED5C-45D8-90CA-FFBB2EDFAE2C}"/>
+    <workbookView xWindow="15825" yWindow="900" windowWidth="14355" windowHeight="10800" activeTab="1" xr2:uid="{A3056EDA-ED5C-45D8-90CA-FFBB2EDFAE2C}"/>
   </bookViews>
   <sheets>
     <sheet name="CAG needed" sheetId="2" r:id="rId1"/>
@@ -1697,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17F8A52-8600-4165-B276-756AD6606234}">
   <dimension ref="A1:AW36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,15 +3100,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15697D8-31F9-47FC-951E-4A3CA050B990}">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -6881,6 +6891,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F19637432BAAAA4E8B613AD4CF549CCD" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1a882fa068e99a90637f35d72ee4199">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f35accf0-cd8f-4670-ac72-d44f2085032d" xmlns:ns4="95507c7c-a837-40bb-8a3d-470d6a1609d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9631af341c2920228165fa301a4a4d8" ns3:_="" ns4:_="">
     <xsd:import namespace="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
@@ -7089,15 +7108,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F7A9799-6172-49A4-97D3-F54069957490}">
   <ds:schemaRefs>
@@ -7116,6 +7126,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D7543C-C9B4-44F7-8DEB-9613BE2D178C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6297254-0AB4-40C6-917E-17F432F90510}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7132,12 +7150,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23D7543C-C9B4-44F7-8DEB-9613BE2D178C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>